<commit_message>
add developmentset and testset
</commit_message>
<xml_diff>
--- a/Samples_clean1.xlsx
+++ b/Samples_clean1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="569">
   <si>
     <t>4XEM VGA Female to Female Adapter</t>
   </si>
@@ -1839,6 +1839,21 @@
   </si>
   <si>
     <t>Premium</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>remium</t>
+    </r>
     <phoneticPr fontId="16" type="noConversion"/>
   </si>
 </sst>
@@ -2387,7 +2402,7 @@
   <dimension ref="A1:D350"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C163" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -4237,7 +4252,9 @@
       <c r="B169" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C169" s="2"/>
+      <c r="C169" s="22" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="1">

</xml_diff>